<commit_message>
Feat: clean the emails in the db
</commit_message>
<xml_diff>
--- a/files/emails.xlsx
+++ b/files/emails.xlsx
@@ -2487,2758 +2487,2758 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>renatangs@terra.com.br</t>
+          <t xml:space="preserve"> contato@auteminvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@auteminvestimentos.com.br </t>
+          <t xml:space="preserve"> rafael.christiansen@bsideinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rafael.christiansen@bsideinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@bbicapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@bbicapital.com.br </t>
+          <t xml:space="preserve"> contato@zhuinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@zhuinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@blackbridgebr.com </t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@blackbridgebr.com </t>
+          <t xml:space="preserve"> rrodrigues@bsprivate.com </t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rrodrigues@bsprivate.com </t>
+          <t xml:space="preserve"> monica.andrade@budinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t xml:space="preserve"> monica.andrade@budinvest.com.br </t>
+          <t xml:space="preserve"> movimentacao@betaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t xml:space="preserve"> movimentacao@betaai.com.br </t>
+          <t xml:space="preserve"> rogerio.feitosa@bloomcapitalaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rogerio.feitosa@bloomcapitalaai.com.br </t>
+          <t xml:space="preserve"> abartho2017@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t xml:space="preserve"> abartho2017@gmail.com </t>
+          <t xml:space="preserve"> contato@cordierinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@cordierinvestimentos.com.br </t>
+          <t xml:space="preserve"> csiinvestimentos@ig.com.br </t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t xml:space="preserve"> csiinvestimentos@ig.com.br </t>
+          <t xml:space="preserve"> carlos.grigoletti@pacecapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t xml:space="preserve"> carlos.grigoletti@pacecapital.com.br </t>
+          <t xml:space="preserve"> contato@convexainvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@convexainvestimentos.com </t>
+          <t xml:space="preserve"> danilobatara@deltaflow.com.br </t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t xml:space="preserve"> danilobatara@deltaflow.com.br </t>
+          <t xml:space="preserve"> augusto.bortolon@docinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t xml:space="preserve"> augusto.bortolon@docinvestimentos.com.br </t>
+          <t xml:space="preserve"> gabriel@dominvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gabriel@dominvestimentos.com.br </t>
+          <t xml:space="preserve"> joao@delfosinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t xml:space="preserve"> joao@delfosinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@drivecapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@drivecapital.com.br </t>
+          <t xml:space="preserve"> bdecourt@everestaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>rodrigo.ganancia@cravacapital.com.br</t>
+          <t xml:space="preserve"> institucional@ewzcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bdecourt@everestaai.com.br </t>
+          <t xml:space="preserve"> atendimento@engageinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t xml:space="preserve"> institucional@ewzcapital.com.br </t>
+          <t xml:space="preserve"> fidus@fidusinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@engageinvest.com.br </t>
+          <t xml:space="preserve"> pedro@forevercapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fidus@fidusinvest.com.br </t>
+          <t xml:space="preserve"> rodrigo@futureinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t xml:space="preserve"> pedro@forevercapital.com.br </t>
+          <t xml:space="preserve"> fmg@g2investimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rodrigo@futureinvest.com.br </t>
+          <t xml:space="preserve"> CARDOSO@GENNESYS.COM </t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fmg@g2investimentos.com.br </t>
+          <t xml:space="preserve"> Humberto.Vallone@galapagoscapital.com </t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CARDOSO@GENNESYS.COM </t>
+          <t xml:space="preserve"> contato@grcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Humberto.Vallone@galapagoscapital.com </t>
+          <t xml:space="preserve"> rodrigo@gtcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@grcapital.com.br </t>
+          <t xml:space="preserve"> administrativo@gueltinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rodrigo@gtcapital.com.br </t>
+          <t xml:space="preserve"> contato@gwminvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t xml:space="preserve"> administrativo@gueltinvestimentos.com.br </t>
+          <t xml:space="preserve"> christianhino@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@gwminvest.com.br </t>
+          <t xml:space="preserve"> haus@hausinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t xml:space="preserve"> christianhino@hotmail.com </t>
+          <t xml:space="preserve"> atendimento@hautinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t xml:space="preserve"> haus@hausinvest.com.br </t>
+          <t xml:space="preserve"> helcio.aguiar@hautinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@hautinvestimentos.com.br </t>
+          <t xml:space="preserve"> integra@integraalianca.com.br </t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t xml:space="preserve"> helcio.aguiar@hautinvestimentos.com.br </t>
+          <t xml:space="preserve"> reinaldo@integralinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t xml:space="preserve"> integra@integraalianca.com.br </t>
+          <t xml:space="preserve"> keliuda@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t xml:space="preserve"> reinaldo@integralinvest.com.br </t>
+          <t xml:space="preserve"> garcia@itajubainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t xml:space="preserve"> keliuda@hotmail.com </t>
+          <t xml:space="preserve"> iwm@iwm.com.br </t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t xml:space="preserve"> garcia@itajubainvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@jacarandainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t xml:space="preserve"> iwm@iwm.com.br </t>
+          <t xml:space="preserve"> comercial@jbninvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@jacarandainvestimentos.com.br </t>
+          <t xml:space="preserve"> cloves@kazacapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t xml:space="preserve"> comercial@jbninvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@sincra.com.br </t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cloves@kazacapital.com.br </t>
+          <t xml:space="preserve"> poliana@kirainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>osmar.mendes@cravacapital.com.br</t>
+          <t xml:space="preserve"> rafael.sanches@kronecapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@sincra.com.br </t>
+          <t xml:space="preserve"> contato@legendinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t xml:space="preserve"> poliana@kirainvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@lifetimeinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rafael.sanches@kronecapital.com.br </t>
+          <t xml:space="preserve"> contato@lineinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@legendinvestimentos.com.br </t>
+          <t xml:space="preserve"> felipe.moraes@liv.capital </t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@lifetimeinvest.com.br </t>
+          <t xml:space="preserve"> contato@lotuscapitalbr.com </t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@lineinvest.com.br </t>
+          <t xml:space="preserve"> LR@LRinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t xml:space="preserve"> felipe.moraes@liv.capital </t>
+          <t xml:space="preserve"> legacy@legacyinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@lotuscapitalbr.com </t>
+          <t xml:space="preserve"> ouvidoria@btgpactual.com </t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LR@LRinvest.com.br </t>
+          <t xml:space="preserve"> adm@m1investimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t xml:space="preserve"> legacy@legacyinvestimentos.com.br </t>
+          <t xml:space="preserve"> eduardo@manacainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ouvidoria@btgpactual.com </t>
+          <t xml:space="preserve"> contato@monitorinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t xml:space="preserve"> adm@m1investimentos.com.br </t>
+          <t xml:space="preserve"> atendimento@menthor.com.vc </t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t xml:space="preserve"> eduardo@manacainvestimentos.com.br </t>
+          <t xml:space="preserve"> daniley@metodoinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@monitorinvestimentos.com.br </t>
+          <t xml:space="preserve"> marcelo.morroni@mgminvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@menthor.com.vc </t>
+          <t xml:space="preserve"> chakmati@mhinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t xml:space="preserve"> daniley@metodoinvestimentos.com.br </t>
+          <t xml:space="preserve"> fernandamoritz@mitb.com.br </t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t xml:space="preserve"> marcelo.morroni@mgminvestimentos.com.br </t>
+          <t xml:space="preserve"> didoramiro@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t xml:space="preserve"> chakmati@mhinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@momentoinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fernandamoritz@mitb.com.br </t>
+          <t xml:space="preserve"> paulo.secco@montealtoinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t xml:space="preserve"> didoramiro@gmail.com </t>
+          <t xml:space="preserve"> fernanda.ramos@mundialinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>circe.machado@cw7aai.com.br</t>
+          <t xml:space="preserve"> ecampos@maisaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>circemachado@yahoo.com</t>
+          <t xml:space="preserve"> relefant@mazalaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>lucas.baron@darental.com.br</t>
+          <t xml:space="preserve"> DANIEL@NOZINVESTIMENTOS.COM.BR </t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@momentoinvest.com.br </t>
+          <t xml:space="preserve"> arthur@netunoinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t xml:space="preserve"> paulo.secco@montealtoinvest.com.br </t>
+          <t xml:space="preserve"> gomesbertolazzo@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fernanda.ramos@mundialinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@octocapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ecampos@maisaai.com.br </t>
+          <t xml:space="preserve"> vinicius.assis@onixcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t xml:space="preserve"> relefant@mazalaai.com.br </t>
+          <t xml:space="preserve"> maicon.melo@otinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DANIEL@NOZINVESTIMENTOS.COM.BR </t>
+          <t xml:space="preserve"> LUIZ.NAZARETH@GMAIL.COM </t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t xml:space="preserve"> arthur@netunoinvestimentos.com.br </t>
+          <t xml:space="preserve"> alessandro.mavignier@oceanoinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gomesbertolazzo@gmail.com </t>
+          <t xml:space="preserve"> Jonas.vicente@investomega.com.br </t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@octocapital.com.br </t>
+          <t xml:space="preserve"> francisco@oneinv.com </t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t xml:space="preserve"> vinicius.assis@onixcapital.com.br </t>
+          <t xml:space="preserve"> contato@pacecapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t xml:space="preserve"> maicon.melo@otinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@panoramainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LUIZ.NAZARETH@GMAIL.COM </t>
+          <t xml:space="preserve"> kirlisson@performe.com.br </t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t xml:space="preserve"> alessandro.mavignier@oceanoinvestimentos.com.br </t>
+          <t xml:space="preserve"> atendimento@perspective.com.br </t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Jonas.vicente@investomega.com.br </t>
+          <t xml:space="preserve"> eg@pfinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t xml:space="preserve"> francisco@oneinv.com </t>
+          <t xml:space="preserve"> rafael.marques@ccninvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@pacecapital.com.br </t>
+          <t xml:space="preserve"> jansen@plentyinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@panoramainvest.com.br </t>
+          <t xml:space="preserve"> contato@pranainvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t xml:space="preserve"> kirlisson@performe.com.br </t>
+          <t xml:space="preserve"> marcos@profittoinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@perspective.com.br </t>
+          <t xml:space="preserve"> jdc@proposito-cap.com </t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>henrique.novais@darental.com.br</t>
+          <t xml:space="preserve"> pvi@pviinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t xml:space="preserve"> eg@pfinvest.com.br </t>
+          <t xml:space="preserve"> contato@potenzacapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rafael.marques@ccninvest.com.br </t>
+          <t xml:space="preserve"> contato@prosperidadeinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t xml:space="preserve"> jansen@plentyinvestimentos.com.br </t>
+          <t xml:space="preserve"> investimentos@raulcarvalhoiv.com.br </t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@pranainvestimentos.com </t>
+          <t xml:space="preserve"> nathaniel@regatainvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t xml:space="preserve"> marcos@profittoinvestimentos.com.br </t>
+          <t xml:space="preserve"> bruno.ismar@renovainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t xml:space="preserve"> jdc@proposito-cap.com </t>
+          <t xml:space="preserve"> atendimento@rubiinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t xml:space="preserve"> pvi@pviinvestimentos.com.br </t>
+          <t xml:space="preserve"> caioesteves@safirainvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@potenzacapital.com.br </t>
+          <t xml:space="preserve"> contato@seedpar.com.br </t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@prosperidadeinvest.com.br </t>
+          <t xml:space="preserve"> institucional@segmentobsb.com.br </t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t xml:space="preserve"> investimentos@raulcarvalhoiv.com.br </t>
+          <t xml:space="preserve"> contato@sigmainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t xml:space="preserve"> nathaniel@regatainvestimentos.com </t>
+          <t xml:space="preserve"> gabriel.paiva@skginvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bruno.ismar@renovainvest.com.br </t>
+          <t xml:space="preserve"> jorny@slrinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@rubiinvestimentos.com.br </t>
+          <t xml:space="preserve"> investimentos@pluginvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t xml:space="preserve"> caioesteves@safirainvestimentos.com </t>
+          <t xml:space="preserve"> isabeladellatorre@swminvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@seedpar.com.br </t>
+          <t xml:space="preserve"> angelica@taggart.com.br </t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t xml:space="preserve"> institucional@segmentobsb.com.br </t>
+          <t xml:space="preserve"> contato@terosinvest.com </t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@sigmainvest.com.br </t>
+          <t xml:space="preserve"> contato@thehill.capital </t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t xml:space="preserve"> gabriel.paiva@skginvestimentos.com.br </t>
+          <t xml:space="preserve"> joaoneto@topinvgroup.com </t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t xml:space="preserve"> jorny@slrinvestimentos.com.br </t>
+          <t xml:space="preserve"> wilson@unifinance.com.br </t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t xml:space="preserve"> investimentos@pluginvestimentos.com.br </t>
+          <t xml:space="preserve"> carolina.araujo@ushuaiainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t xml:space="preserve"> isabeladellatorre@swminvest.com.br </t>
+          <t xml:space="preserve"> fbrant@refraninvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t xml:space="preserve"> angelica@taggart.com.br </t>
+          <t xml:space="preserve"> contato@vertenteaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@terosinvest.com </t>
+          <t xml:space="preserve"> contato@veedha.com.br </t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@thehill.capital </t>
+          <t xml:space="preserve"> juliana.menon@vgvinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t xml:space="preserve"> joaoneto@topinvgroup.com </t>
+          <t xml:space="preserve"> rm@viddacapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t xml:space="preserve"> wilson@unifinance.com.br </t>
+          <t xml:space="preserve"> venice@veniceinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t xml:space="preserve"> carolina.araujo@ushuaiainvestimentos.com.br </t>
+          <t xml:space="preserve"> micheliif@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fbrant@refraninvest.com.br </t>
+          <t xml:space="preserve"> contato@wavecap.com.br </t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@vertenteaai.com.br </t>
+          <t xml:space="preserve"> andre@wayinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@veedha.com.br </t>
+          <t xml:space="preserve"> guilherme@wgcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>luiza@diamantinainvestimentos.com.br</t>
+          <t xml:space="preserve"> ADMINISTRATIVO@WISEAAI.COM.BR </t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t xml:space="preserve"> juliana.menon@vgvinvest.com.br </t>
+          <t xml:space="preserve"> contato@wtacapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rm@viddacapital.com.br </t>
+          <t xml:space="preserve"> Contato@wertinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t xml:space="preserve"> venice@veniceinvest.com.br </t>
+          <t xml:space="preserve"> Rodrigo.borba@westinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t xml:space="preserve"> micheliif@hotmail.com </t>
+          <t xml:space="preserve"> atendimento@ybotirama.com </t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@wavecap.com.br </t>
+          <t xml:space="preserve"> antoni@zbnivestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t xml:space="preserve"> andre@wayinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@zunar.com.br </t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t xml:space="preserve"> guilherme@wgcapital.com.br </t>
+          <t xml:space="preserve">marcela@vkpartners.com.br </t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ADMINISTRATIVO@WISEAAI.COM.BR </t>
+          <t xml:space="preserve">leonardo.fernandes@exclusiveinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@wtacapital.com.br </t>
+          <t xml:space="preserve">cecilio.costa@mhydasinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Contato@wertinvestimentos.com.br </t>
+          <t xml:space="preserve">vitorpacifico@capitalinvestimento.com.br; francisco.ribeiro@capitalinvestimento.com.br </t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rodrigo.borba@westinvestimentos.com.br </t>
+          <t xml:space="preserve">alvaro@adinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@ybotirama.com </t>
+          <t xml:space="preserve">joao@joaoallora.com.br </t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t xml:space="preserve"> antoni@zbnivestimentos.com.br </t>
+          <t xml:space="preserve">viviane@tmrmais.com.br </t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@zunar.com.br </t>
+          <t xml:space="preserve">atendimento@lfrinvestimentos.com.br ; leonardo.rodrigues@lfrinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t xml:space="preserve">marcela@vkpartners.com.br </t>
+          <t xml:space="preserve">volnei.gomes@pienzainvestimentos.com.br; vaniasavi@pienzainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t xml:space="preserve">leonardo.fernandes@exclusiveinvestimentos.com.br </t>
+          <t xml:space="preserve">juliano@m9p.com.br </t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t xml:space="preserve">cecilio.costa@mhydasinvestimentos.com </t>
+          <t xml:space="preserve">thiago@vokseinvest.com.br; allan@vokseinvest.com.br gregorio@vokseinvest.com.br charline@vokseinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t xml:space="preserve">vitorpacifico@capitalinvestimento.com.br; francisco.ribeiro@capitalinvestimento.com.br </t>
+          <t xml:space="preserve">thiago@nex1investimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t xml:space="preserve">alvaro@adinvestimentos.com.br </t>
+          <t xml:space="preserve">hamyrez.barbosa@akivcinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t xml:space="preserve">joao@joaoallora.com.br </t>
+          <t xml:space="preserve">raphael.mendes@akivainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t xml:space="preserve">viviane@tmrmais.com.br </t>
+          <t xml:space="preserve">bianchini@alappinvest.com </t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t xml:space="preserve">atendimento@lfrinvestimentos.com.br ; leonardo.rodrigues@lfrinvestimentos.com.br </t>
+          <t xml:space="preserve">jeferson@aligninvest.com.br ; guilhermeolinto_aai@outlook.com; fabiola@aligninvest.com.br; hellen@aligninvest.com.br; vera@aligninvest.com.br; mariadapenha@aligninvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t xml:space="preserve">volnei.gomes@pienzainvestimentos.com.br; vaniasavi@pienzainvestimentos.com.br </t>
+          <t xml:space="preserve">debora@allorainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t xml:space="preserve">juliano@m9p.com.br </t>
+          <t xml:space="preserve">allux@alluxinvestimentos.com; ernesto@alluxinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t xml:space="preserve">thiago@vokseinvest.com.br; allan@vokseinvest.com.br gregorio@vokseinvest.com.br charline@vokseinvest.com.br </t>
+          <t xml:space="preserve">a.latina@terra.com.br </t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t xml:space="preserve">thiago@nex1investimentos.com.br </t>
+          <t xml:space="preserve">fargeti@slw.com.br </t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t xml:space="preserve">hamyrez.barbosa@akivcinvest.com.br </t>
+          <t xml:space="preserve">antoniofgb@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t xml:space="preserve">raphael.mendes@akivainvest.com.br </t>
+          <t xml:space="preserve">tony@tonycoelho.com.br </t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t xml:space="preserve">bianchini@alappinvest.com </t>
+          <t xml:space="preserve">lfrazatto@yahoo.com </t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t xml:space="preserve">jeferson@aligninvest.com.br ; guilhermeolinto_aai@outlook.com; fabiola@aligninvest.com.br; hellen@aligninvest.com.br; vera@aligninvest.com.br; mariadapenha@aligninvest.com.br </t>
+          <t xml:space="preserve">abreu@arrecifeaai.com.br; carlosvalle@arrecifeaai.com.br; matheus@arrecifeaai.com.br; pedro@arrecifeaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t xml:space="preserve">debora@allorainvestimentos.com.br </t>
+          <t xml:space="preserve">gereci@bgrcapital.com.br ; rodrigo@bgrcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t xml:space="preserve">allux@alluxinvestimentos.com; ernesto@alluxinvestimentos.com </t>
+          <t xml:space="preserve">jose.valdoir@blackross.com.br; sgiuntini@blackross.com.br </t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t xml:space="preserve">a.latina@terra.com.br </t>
+          <t xml:space="preserve">g.caiuby.novaes@uol.com.br </t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t xml:space="preserve">fargeti@slw.com.br </t>
+          <t xml:space="preserve">gustavoscabral83@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t xml:space="preserve">antoniofgb@hotmail.com </t>
+          <t xml:space="preserve">daniel@calipeinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t xml:space="preserve">tony@tonycoelho.com.br </t>
+          <t xml:space="preserve">ctaphilipp@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t xml:space="preserve">lfrazatto@yahoo.com </t>
+          <t xml:space="preserve">administrativo@conquestconsultoria.com </t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>nuno.cruz@estorilinvestimentos.com.br</t>
+          <t xml:space="preserve">francisco.vaz@dapesinvestimentos.com.br ; alfredo@dapesinvestimentos.com.br; rodrigo@dapesinvestimentos.com.br; joão@dapesinvestimentos.com.br; henrique@dapesinvestimentos.com.br; felipe@dapesinvestimentos.com.br; raul@dapesinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t xml:space="preserve">abreu@arrecifeaai.com.br; carlosvalle@arrecifeaai.com.br; matheus@arrecifeaai.com.br; pedro@arrecifeaai.com.br </t>
+          <t xml:space="preserve">denerp.ag@gmail.com  </t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t xml:space="preserve">gereci@bgrcapital.com.br ; rodrigo@bgrcapital.com.br </t>
+          <t xml:space="preserve">sibelle@diamantinainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t xml:space="preserve">jose.valdoir@blackross.com.br; sgiuntini@blackross.com.br </t>
+          <t xml:space="preserve">socios@dnainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t xml:space="preserve">g.caiuby.novaes@uol.com.br </t>
+          <t xml:space="preserve">henrique@aai.loteinvest.com; fernando@aai.loteinvest.com </t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t xml:space="preserve">gustavoscabral83@gmail.com </t>
+          <t xml:space="preserve">ctn@egsinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t xml:space="preserve">daniel@calipeinvestimentos.com </t>
+          <t xml:space="preserve">elizabetholivo.bnpp@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t xml:space="preserve">ctaphilipp@gmail.com </t>
+          <t xml:space="preserve">ennardelli@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t xml:space="preserve">administrativo@conquestconsultoria.com </t>
+          <t xml:space="preserve">isidoriosimoes@atuacaopart.com.br </t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t xml:space="preserve">francisco.vaz@dapesinvestimentos.com.br ; alfredo@dapesinvestimentos.com.br; rodrigo@dapesinvestimentos.com.br; joão@dapesinvestimentos.com.br; henrique@dapesinvestimentos.com.br; felipe@dapesinvestimentos.com.br; raul@dapesinvestimentos.com.br </t>
+          <t xml:space="preserve">alexandre.abreu@estruturalinvestimentos.com.br; fernando.zanoli@estruturalinvestimentos.com.br; camila.lessa@estruturalinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t xml:space="preserve">denerp.ag@gmail.com  </t>
+          <t xml:space="preserve">gustavo.ribolli@einv.com.br; admilson@einvcom.br; gilberto.gumieri@einv.com.br; </t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t xml:space="preserve">sibelle@diamantinainvestimentos.com.br </t>
+          <t xml:space="preserve">contato@facilitainveste.com.br | julio.basilio@facilitainveste.com.br |rgonzalez@facilitainveste.com.br | leonardo.lewandowski@facilitainveste.com.br | rafael.pianca@facilitainveste.com.br | moacir.arimura@facilitainveste.com.br </t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t xml:space="preserve">socios@dnainvest.com.br </t>
+          <t xml:space="preserve">marcello.predolin@flapcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t xml:space="preserve">henrique@aai.loteinvest.com; fernando@aai.loteinvest.com </t>
+          <t xml:space="preserve">flavia.nunnes@nunnesinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t xml:space="preserve">ctn@egsinvestimentos.com.br </t>
+          <t xml:space="preserve">eliel.lins@mundoinvestimentos.com.br; luana.moreira@mundoinvestimentos.com.br; maico.bosi@mundoinvestimentos.com.br; mauricius.munhoz@mundoinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t xml:space="preserve">elizabetholivo.bnpp@hotmail.com </t>
+          <t xml:space="preserve">renato.sabino@fmbinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t xml:space="preserve">ennardelli@gmail.com </t>
+          <t xml:space="preserve">fbrant@refraninvest.com.br; carolferreira@refraninvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t xml:space="preserve">isidoriosimoes@atuacaopart.com.br </t>
+          <t xml:space="preserve">eilatinvestimentos@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t xml:space="preserve">alexandre.abreu@estruturalinvestimentos.com.br; fernando.zanoli@estruturalinvestimentos.com.br; camila.lessa@estruturalinvestimentos.com.br </t>
+          <t xml:space="preserve">gdias@guideinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t xml:space="preserve">gustavo.ribolli@einv.com.br; admilson@einvcom.br; gilberto.gumieri@einv.com.br; </t>
+          <t xml:space="preserve">paulo@goldrock.com.br; </t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t xml:space="preserve">contato@facilitainveste.com.br | julio.basilio@facilitainveste.com.br |rgonzalez@facilitainveste.com.br | leonardo.lewandowski@facilitainveste.com.br | rafael.pianca@facilitainveste.com.br | moacir.arimura@facilitainveste.com.br </t>
+          <t xml:space="preserve">guilherme.moraes@grmcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t xml:space="preserve">marcello.predolin@flapcapital.com.br </t>
+          <t xml:space="preserve">gwm@gwmpx.com </t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t xml:space="preserve">flavia.nunnes@nunnesinvestimentos.com.br </t>
+          <t xml:space="preserve">luiz@helmanadvisor.com.br </t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t xml:space="preserve">eliel.lins@mundoinvestimentos.com.br; luana.moreira@mundoinvestimentos.com.br; maico.bosi@mundoinvestimentos.com.br; mauricius.munhoz@mundoinvestimentos.com.br </t>
+          <t xml:space="preserve">luiz@investgroup.com.br; pellin@investigroup.com.br </t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t xml:space="preserve">renato.sabino@fmbinvest.com.br </t>
+          <t xml:space="preserve">rsoggia@itajubainvestimentos.com.br ; pbiase@itajubainvestimentos.com.br ; mizael@itajubainvestimentos.com.br ; bqueima@itajubainvestimentos.com.br ; garcia@itajubainvestimentos.com.br ; filipe@itajubainvestimentos.com.br ; agnaldo.andrade@itajubainvestimentos.com.br ; lcamozzato@itajubainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t xml:space="preserve">fbrant@refraninvest.com.br; carolferreira@refraninvest.com.br </t>
+          <t xml:space="preserve">jacques.abram@abramaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t xml:space="preserve">eilatinvestimentos@gmail.com </t>
+          <t xml:space="preserve">maikel@jacobcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t xml:space="preserve">gdias@guideinvestimentos.com.br </t>
+          <t xml:space="preserve">jbatistaautonomosjosecarlos@gmail.com; jbatistaautonomos.gabriel@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t xml:space="preserve">paulo@goldrock.com.br; </t>
+          <t xml:space="preserve">leon@jlvinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t xml:space="preserve">guilherme.moraes@grmcapital.com.br </t>
+          <t xml:space="preserve">jminvestimentos@jotam.com.br </t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t xml:space="preserve">gwm@gwmpx.com </t>
+          <t xml:space="preserve">trmontenegro@uol.com.br </t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t xml:space="preserve">luiz@helmanadvisor.com.br </t>
+          <t xml:space="preserve">ilan@lanix.com.br </t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t xml:space="preserve">luiz@investgroup.com.br; pellin@investigroup.com.br </t>
+          <t xml:space="preserve">vinicios@lucrarinvestimentos.com.br; stephan@lucrarnvestimentos.com.br; cleodutra@lucrarinvestimentos.com.br; giovano@lucrarinvestimentos.com.br; </t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t xml:space="preserve">rsoggia@itajubainvestimentos.com.br ; pbiase@itajubainvestimentos.com.br ; mizael@itajubainvestimentos.com.br ; bqueima@itajubainvestimentos.com.br ; garcia@itajubainvestimentos.com.br ; filipe@itajubainvestimentos.com.br ; agnaldo.andrade@itajubainvestimentos.com.br ; lcamozzato@itajubainvestimentos.com.br </t>
+          <t xml:space="preserve">fernanda.abrhao@lusinvest.com.br; keila.clemente@lusinvest.com.br; liliana.sadi@lusinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t xml:space="preserve">jacques.abram@abramaai.com.br </t>
+          <t xml:space="preserve">rafael.marques@matriceinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t xml:space="preserve">maikel@jacobcapital.com.br </t>
+          <t xml:space="preserve">aily@neovalorinvestimentos.com; carlos@neovalorinvestimentos.com; juliana@neovalorinvestimentos.com; matheus@neovalorinvestimentos.comtimoteo@neovalorinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t xml:space="preserve">jbatistaautonomosjosecarlos@gmail.com; jbatistaautonomos.gabriel@gmail.com </t>
+          <t xml:space="preserve">eduardo@newestate.com.br </t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t xml:space="preserve">leon@jlvinvestimentos.com.br </t>
+          <t xml:space="preserve">amandadiniz@octocapital.com.br; mariananery@octocapital.com.br; gabriel@octocapital.com.br; lucas@octocapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t xml:space="preserve">jminvestimentos@jotam.com.br </t>
+          <t xml:space="preserve">kelly@pinvesti.com.br </t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t xml:space="preserve">trmontenegro@uol.com.br </t>
+          <t xml:space="preserve">kirlisson@performance.com.br </t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t xml:space="preserve">ilan@lanix.com.br </t>
+          <t xml:space="preserve">enzo@pfiaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t xml:space="preserve">vinicios@lucrarinvestimentos.com.br; stephan@lucrarnvestimentos.com.br; cleodutra@lucrarinvestimentos.com.br; giovano@lucrarinvestimentos.com.br; </t>
+          <t xml:space="preserve">contato@phiinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>rui.pinto@estorilinvestimentos.com.br</t>
+          <t xml:space="preserve">bruno.zanuzzo@podiuminvest.com.br; larissa.pereira@podiuminvest.com.br; ian.gadelha@podiuminvest.com.br; elton.cruz@podiumi.com.br </t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>contato@everestaai.com.br</t>
+          <t xml:space="preserve">frederico@prioreinvestimentos.com.br; rodrigo@prioreinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>guilhermo@experinvestimentos.com</t>
+          <t xml:space="preserve">anapaula@privateaai.com.br; fabiano@privateaai.com.br; rinaldo@privateaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t xml:space="preserve">fernanda.abrhao@lusinvest.com.br; keila.clemente@lusinvest.com.br; liliana.sadi@lusinvest.com.br </t>
+          <t xml:space="preserve">andre.shinohara@prosperitat.com.br; marcelo.vaz@prosperitat.com.br </t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t xml:space="preserve">rafael.marques@matriceinvest.com.br </t>
+          <t xml:space="preserve">renato_roizenblit@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t xml:space="preserve">aily@neovalorinvestimentos.com; carlos@neovalorinvestimentos.com; juliana@neovalorinvestimentos.com; matheus@neovalorinvestimentos.comtimoteo@neovalorinvestimentos.com </t>
+          <t xml:space="preserve">daniel@razoesinvest.com.br; marcelo@razoesparainvestir.com.br </t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t xml:space="preserve">eduardo@newestate.com.br </t>
+          <t xml:space="preserve">sirlene@rhyalinvestimentos.com.br; cleverson@rhyalinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t xml:space="preserve">amandadiniz@octocapital.com.br; mariananery@octocapital.com.br; gabriel@octocapital.com.br; lucas@octocapital.com.br </t>
+          <t xml:space="preserve">francisco.giannocaro@guideinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t xml:space="preserve">kelly@pinvesti.com.br </t>
+          <t xml:space="preserve">alexandre.mourani@severa.com.br </t>
         </is>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t xml:space="preserve">kirlisson@performance.com.br </t>
+          <t xml:space="preserve">sol_nascente@uol.com.br </t>
         </is>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t xml:space="preserve">enzo@pfiaai.com.br </t>
+          <t xml:space="preserve">aai@pluginvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t xml:space="preserve">contato@phiinvestimentos.com.br </t>
+          <t xml:space="preserve">carlos.castro@superrico.com.br </t>
         </is>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t xml:space="preserve">bruno.zanuzzo@podiuminvest.com.br; larissa.pereira@podiuminvest.com.br; ian.gadelha@podiuminvest.com.br; elton.cruz@podiumi.com.br </t>
+          <t xml:space="preserve">risco@unifinance.com.br </t>
         </is>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t xml:space="preserve">frederico@prioreinvestimentos.com.br; rodrigo@prioreinvestimentos.com.br </t>
+          <t xml:space="preserve">leonardo@uprealinvestimentos.com.br; luislafratta@uprealinvestimentos.com.br; rodrigo@uprealinvestimentos.com.br; david@uprealinvestimentos.com.br; rafael@uprealinvestimentos.com.br; simone@uprealinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t xml:space="preserve">anapaula@privateaai.com.br; fabiano@privateaai.com.br; rinaldo@privateaai.com.br </t>
+          <t xml:space="preserve">marcio.leandro@upstock.com.br </t>
         </is>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t xml:space="preserve">andre.shinohara@prosperitat.com.br; marcelo.vaz@prosperitat.com.br </t>
+          <t xml:space="preserve">diogo.calmon@valeverdeinvest.com.br ; gabriela@otbinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t xml:space="preserve">renato_roizenblit@hotmail.com </t>
+          <t xml:space="preserve">vega@vegagp.com.br; vega@vega.adm.br </t>
         </is>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t xml:space="preserve">daniel@razoesinvest.com.br; marcelo@razoesparainvestir.com.br </t>
+          <t xml:space="preserve">juliana@vgvaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t xml:space="preserve">sirlene@rhyalinvestimentos.com.br; cleverson@rhyalinvestimentos.com.br </t>
+          <t xml:space="preserve">emiimai@vmpg.com.br </t>
         </is>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t xml:space="preserve">francisco.giannocaro@guideinvestimentos.com.br </t>
+          <t xml:space="preserve">paulo.cunha@zeusinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t xml:space="preserve">alexandre.mourani@severa.com.br </t>
+          <t>nathanael@a7solucoes.com</t>
         </is>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t xml:space="preserve">sol_nascente@uol.com.br </t>
+          <t>nathanael@a7solucoesfinanceiras.com</t>
         </is>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>mirele@experinvestimentos.com</t>
+          <t>kaue@al7invest.com.br</t>
         </is>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>ayrton.medeiros@fiere.com.br</t>
+          <t>contato@akivcinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t xml:space="preserve">aai@pluginvest.com.br </t>
+          <t>hamyrez@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t xml:space="preserve">carlos.castro@superrico.com.br </t>
+          <t>alexandresandoval@alluxinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t xml:space="preserve">risco@unifinance.com.br </t>
+          <t>ronaldobella@alluxinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t xml:space="preserve">leonardo@uprealinvestimentos.com.br; luislafratta@uprealinvestimentos.com.br; rodrigo@uprealinvestimentos.com.br; david@uprealinvestimentos.com.br; rafael@uprealinvestimentos.com.br; simone@uprealinvestimentos.com.br </t>
+          <t>ernesto@smarting.com.br</t>
         </is>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t xml:space="preserve">marcio.leandro@upstock.com.br </t>
+          <t>contato@alpinaaai.com.br</t>
         </is>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t xml:space="preserve">diogo.calmon@valeverdeinvest.com.br ; gabriela@otbinvest.com.br </t>
+          <t>fernando@alpinaaai.com.br</t>
         </is>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>Admilson@fiere.com.br</t>
+          <t>fpalmendra@alpinaaai.com.br</t>
         </is>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>alex.orlandini@fiere.com.br</t>
+          <t>caio.mathias@arkinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>anderson.ribeiro@fiere.com.br</t>
+          <t>contato@arkinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>carla.barros@fiere.com.br</t>
+          <t>daniel.granuzzo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>gabriel.zaiden@fiere.com.br</t>
+          <t>Leonardo.ferreira@arkinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>gustavo.medina@fiere.com.br</t>
+          <t>frpeccini@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="inlineStr">
         <is>
-          <t>wesley.dias@fiere.com.br</t>
+          <t>adm@astecainvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="inlineStr">
         <is>
-          <t>aldenorpessoa@financademy.com</t>
+          <t>denis@astecainvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="inlineStr">
         <is>
-          <t>paulomarques@financademy.com</t>
+          <t>operacional@astecainvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="533">
       <c r="A533" t="inlineStr">
         <is>
-          <t>felipe.noer@fragatainvestimentos.com.br</t>
+          <t>rogerio@astecainvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="534">
       <c r="A534" t="inlineStr">
         <is>
-          <t>martina.patussi@fragatainvestimentos.com.br</t>
+          <t>leonardo@austriacap.com.br</t>
         </is>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t xml:space="preserve">vega@vegagp.com.br; vega@vega.adm.br </t>
+          <t>bruna@austriacap.com.br</t>
         </is>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="inlineStr">
         <is>
-          <t xml:space="preserve">juliana@vgvaai.com.br </t>
+          <t>gustavo.lessa@austriacap.com.br</t>
         </is>
       </c>
     </row>
     <row r="537">
       <c r="A537" t="inlineStr">
         <is>
-          <t xml:space="preserve">emiimai@vmpg.com.br </t>
+          <t>banestesinvestimentos@banestes.com.br</t>
         </is>
       </c>
     </row>
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t xml:space="preserve">paulo.cunha@zeusinvestimentos.com.br </t>
+          <t>ctjesus@banestes.com.br</t>
         </is>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>nathanael@a7solucoes.com</t>
+          <t>leomarcampos@banestes.com.br</t>
         </is>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>nathanael@a7solucoesfinanceiras.com</t>
+          <t>boris@brgi.com.br</t>
         </is>
       </c>
     </row>
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>kaue@al7invest.com.br</t>
+          <t>andre@bridgeinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>contato@akivcinvest.com.br</t>
+          <t>dayan@bridgeinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>hamyrez@hotmail.com</t>
+          <t>atendimento@bridgeinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="544">
       <c r="A544" t="inlineStr">
         <is>
-          <t>alexandresandoval@alluxinvestimentos.com.br</t>
+          <t>pedro@bridgeinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="545">
       <c r="A545" t="inlineStr">
         <is>
-          <t>ronaldobella@alluxinvestimentos.com.br</t>
+          <t>keverson@bullbearcapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="546">
       <c r="A546" t="inlineStr">
         <is>
-          <t>ernesto@smarting.com.br</t>
+          <t>rodrigopaula@contemporaneocapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="inlineStr">
         <is>
-          <t>contato@alpinaaai.com.br</t>
+          <t>henrique.hellas@continuumprivate.com.br</t>
         </is>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>fernando@alpinaaai.com.br</t>
+          <t>joao.limeira@continuumprivate.com.br</t>
         </is>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="inlineStr">
         <is>
-          <t>fpalmendra@alpinaaai.com.br</t>
+          <t>alberto.rocha@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="inlineStr">
         <is>
-          <t>caio.mathias@arkinvestimentos.com.br</t>
+          <t>arthur.moraes@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="inlineStr">
         <is>
-          <t>contato@arkinvestimentos.com.br</t>
+          <t>assessoria@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="inlineStr">
         <is>
-          <t>daniel.granuzzo@gmail.com</t>
+          <t>claudio.pereira@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>Leonardo.ferreira@arkinvestimentos.com.br</t>
+          <t>crava@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="inlineStr">
         <is>
-          <t>frpeccini@gmail.com</t>
+          <t>enio.fernando@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="inlineStr">
         <is>
-          <t>adm@astecainvest.com.br</t>
+          <t>rodrigo.souto@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="inlineStr">
         <is>
-          <t>denis@astecainvest.com.br</t>
+          <t>vania.freire@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="inlineStr">
         <is>
-          <t>operacional@astecainvest.com.br</t>
+          <t>rodrigo.ganancia@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="558">
       <c r="A558" t="inlineStr">
         <is>
-          <t>rogerio@astecainvest.com.br</t>
+          <t>osmar.mendes@cravacapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>leonardo@austriacap.com.br</t>
+          <t>circe.machado@cw7aai.com.br</t>
         </is>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>bruna@austriacap.com.br</t>
+          <t>circemachado@yahoo.com</t>
         </is>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>gustavo.lessa@austriacap.com.br</t>
+          <t>lucas.baron@darental.com.br</t>
         </is>
       </c>
     </row>
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>banestesinvestimentos@banestes.com.br</t>
+          <t>henrique.novais@darental.com.br</t>
         </is>
       </c>
     </row>
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>ctjesus@banestes.com.br</t>
+          <t>luiza@diamantinainvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="inlineStr">
         <is>
-          <t>leomarcampos@banestes.com.br</t>
+          <t>nuno.cruz@estorilinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="inlineStr">
         <is>
-          <t>boris@brgi.com.br</t>
+          <t>rui.pinto@estorilinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="inlineStr">
         <is>
-          <t>andre@bridgeinvest.com.br</t>
+          <t>contato@everestaai.com.br</t>
         </is>
       </c>
     </row>
     <row r="567">
       <c r="A567" t="inlineStr">
         <is>
-          <t>dayan@bridgeinvest.com.br</t>
+          <t>guilhermo@experinvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="568">
       <c r="A568" t="inlineStr">
         <is>
-          <t>atendimento@bridgeinvest.com.br</t>
+          <t>mirele@experinvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="569">
       <c r="A569" t="inlineStr">
         <is>
-          <t>pedro@bridgeinvest.com.br</t>
+          <t>ayrton.medeiros@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="570">
       <c r="A570" t="inlineStr">
         <is>
-          <t>keverson@bullbearcapital.com.br</t>
+          <t>Admilson@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="571">
       <c r="A571" t="inlineStr">
         <is>
-          <t>rodrigopaula@contemporaneocapital.com.br</t>
+          <t>alex.orlandini@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="inlineStr">
         <is>
-          <t>henrique.hellas@continuumprivate.com.br</t>
+          <t>anderson.ribeiro@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="inlineStr">
         <is>
-          <t>joao.limeira@continuumprivate.com.br</t>
+          <t>carla.barros@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>alberto.rocha@cravacapital.com.br</t>
+          <t>gabriel.zaiden@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>arthur.moraes@cravacapital.com.br</t>
+          <t>gustavo.medina@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>assessoria@cravacapital.com.br</t>
+          <t>wesley.dias@fiere.com.br</t>
         </is>
       </c>
     </row>
     <row r="577">
       <c r="A577" t="inlineStr">
         <is>
-          <t>claudio.pereira@cravacapital.com.br</t>
+          <t>aldenorpessoa@financademy.com</t>
         </is>
       </c>
     </row>
     <row r="578">
       <c r="A578" t="inlineStr">
         <is>
-          <t>crava@cravacapital.com.br</t>
+          <t>paulomarques@financademy.com</t>
         </is>
       </c>
     </row>
     <row r="579">
       <c r="A579" t="inlineStr">
         <is>
-          <t>enio.fernando@cravacapital.com.br</t>
+          <t>felipe.noer@fragatainvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="580">
       <c r="A580" t="inlineStr">
         <is>
-          <t>rodrigo.souto@cravacapital.com.br</t>
+          <t>martina.patussi@fragatainvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="581">
       <c r="A581" t="inlineStr">
         <is>
-          <t>vania.freire@cravacapital.com.br</t>
+          <t>danilo.kenji@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="inlineStr">
         <is>
-          <t>danilo.kenji@gadeinvestimentos.com.br</t>
+          <t>douglas.pasquini@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="583">
       <c r="A583" t="inlineStr">
         <is>
-          <t>douglas.pasquini@gadeinvestimentos.com.br</t>
+          <t>joao.cristovao@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>joao.cristovao@gadeinvestimentos.com.br</t>
+          <t>jose.zavatin@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="inlineStr">
         <is>
-          <t>jose.zavatin@gadeinvestimentos.com.br</t>
+          <t xml:space="preserve">jose.zavatin@gadeinvestimentos.com.br&gt; </t>
         </is>
       </c>
     </row>
     <row r="586">
       <c r="A586" t="inlineStr">
         <is>
-          <t xml:space="preserve">jose.zavatin@gadeinvestimentos.com.br&gt; </t>
+          <t>fernando.menolli@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>fernando.menolli@gadeinvestimentos.com.br</t>
+          <t>marcos.biasao@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="588">
       <c r="A588" t="inlineStr">
         <is>
-          <t>marcos.biasao@gadeinvestimentos.com.br</t>
+          <t>mateus.bitencourt@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="589">
       <c r="A589" t="inlineStr">
         <is>
-          <t>mateus.bitencourt@gadeinvestimentos.com.br</t>
+          <t>sergio.oliveira@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="590">
       <c r="A590" t="inlineStr">
         <is>
-          <t>sergio.oliveira@gadeinvestimentos.com.br</t>
+          <t>thiago.moreira@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="inlineStr">
         <is>
-          <t>thiago.moreira@gadeinvestimentos.com.br</t>
+          <t>vinicius.menta@gadeinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="592">
       <c r="A592" t="inlineStr">
         <is>
-          <t>vinicius.menta@gadeinvestimentos.com.br</t>
+          <t>b2bcomercial@genial.com.vc</t>
         </is>
       </c>
     </row>
     <row r="593">
       <c r="A593" t="inlineStr">
         <is>
-          <t>b2bcomercial@genial.com.vc</t>
+          <t>adrianopescada@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="594">
       <c r="A594" t="inlineStr">
         <is>
-          <t>adrianopescada@gmail.com</t>
+          <t>agenteautonomopedro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="595">
       <c r="A595" t="inlineStr">
         <is>
-          <t>agenteautonomopedro@gmail.com</t>
+          <t>antonio.penauri@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>antonio.penauri@gmail.com</t>
+          <t>apsinvest7@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>apsinvest7@gmail.com</t>
+          <t>b2rinvestimentos@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>b2rinvestimentos@gmail.com</t>
+          <t>ballejoalvaro@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>ballejoalvaro@gmail.com</t>
+          <t>cassiobarbosa14@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>cassiobarbosa14@gmail.com</t>
+          <t>cesar.picolo@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="601">
       <c r="A601" t="inlineStr">
         <is>
-          <t>cesar.picolo@gmail.com</t>
+          <t>denielmoraes@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>denielmoraes@gmail.com</t>
+          <t>fernavoli@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>fernavoli@gmail.com</t>
+          <t>fmenesessobreira@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>fmenesessobreira@gmail.com</t>
+          <t>genial.sejacasa@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>genial.sejacasa@gmail.com</t>
+          <t>guilhermelagesvr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>guilhermelagesvr@gmail.com</t>
+          <t>Joelortiz.lehaim@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>Joelortiz.lehaim@gmail.com</t>
+          <t>jose.bolibioaai@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>jose.bolibioaai@gmail.com</t>
+          <t>jozephbrasil@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>jozephbrasil@gmail.com</t>
+          <t>kaueassessor@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>kaueassessor@gmail.com</t>
+          <t>panassoloj@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>panassoloj@gmail.com</t>
+          <t>PAULO.PENAURI@GMAIL.COM</t>
         </is>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>PAULO.PENAURI@GMAIL.COM</t>
+          <t>rodrigodossantospaula@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>rodrigodossantospaula@gmail.com</t>
+          <t>tullio.bonsaver@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>tullio.bonsaver@gmail.com</t>
+          <t>w1968jr@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>w1968jr@gmail.com</t>
+          <t>wimryansp@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>wimryansp@gmail.com</t>
+          <t>joao.martinussi@gridinvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>joao.martinussi@gridinvestimentos.com</t>
+          <t>priscila@gridinvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>priscila@gridinvestimentos.com</t>
+          <t>lucas.rodrigues@grupotgl.com</t>
         </is>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="inlineStr">
         <is>
-          <t>lucas.rodrigues@grupotgl.com</t>
+          <t>harta@harta.capital</t>
         </is>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
         <is>
-          <t>harta@harta.capital</t>
+          <t>aneto@hdginvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="inlineStr">
         <is>
-          <t>aneto@hdginvestimentos.com.br</t>
+          <t>Giovani.pasquali@hefestoinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="inlineStr">
         <is>
-          <t>Giovani.pasquali@hefestoinvestimentos.com.br</t>
+          <t>cintia.advisor@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>cintia.advisor@hotmail.com</t>
+          <t>cmte.aires@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>cmte.aires@hotmail.com</t>
+          <t>danielguisard@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="625">
       <c r="A625" t="inlineStr">
         <is>
-          <t>danielguisard@hotmail.com</t>
+          <t>danilodc40@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>danilodc40@hotmail.com</t>
+          <t>gontijose@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="627">
       <c r="A627" t="inlineStr">
         <is>
-          <t>gontijose@hotmail.com</t>
+          <t>larmonteiro@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="628">
       <c r="A628" t="inlineStr">
         <is>
-          <t>larmonteiro@hotmail.com</t>
+          <t>leoprezotti@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>leoprezotti@hotmail.com</t>
+          <t>mateuslovatte@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="630">
       <c r="A630" t="inlineStr">
         <is>
-          <t>mateuslovatte@hotmail.com</t>
+          <t>rodmanfredini@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="631">
       <c r="A631" t="inlineStr">
         <is>
-          <t>rodmanfredini@hotmail.com</t>
+          <t>sgloyo@hotmail.com</t>
         </is>
       </c>
     </row>
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>sgloyo@hotmail.com</t>
+          <t>mesa@htin.com.br</t>
         </is>
       </c>
     </row>
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>mesa@htin.com.br</t>
+          <t>zarife@icaraiinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t>zarife@icaraiinvestimentos.com.br</t>
+          <t>aislan.tito@ipeinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>aislan.tito@ipeinvest.com.br</t>
+          <t>sergio.loyo@loyopuscapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>sergio.loyo@loyopuscapital.com.br</t>
+          <t>alvaro.castro@maiscapital.net</t>
         </is>
       </c>
     </row>
     <row r="637">
       <c r="A637" t="inlineStr">
         <is>
-          <t>alvaro.castro@maiscapital.net</t>
+          <t>daniel.azevedo@maiscapital.net</t>
         </is>
       </c>
     </row>
     <row r="638">
       <c r="A638" t="inlineStr">
         <is>
-          <t>daniel.azevedo@maiscapital.net</t>
+          <t>atendimento@martelloinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>atendimento@martelloinvestimentos.com.br</t>
+          <t>leandro.biggi@martelloinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>leandro.biggi@martelloinvestimentos.com.br</t>
+          <t>thiago@martelloinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="641">
       <c r="A641" t="inlineStr">
         <is>
-          <t>thiago@martelloinvestimentos.com.br</t>
+          <t>relefant@mazalaai.com.br</t>
         </is>
       </c>
     </row>
     <row r="642">
       <c r="A642" t="inlineStr">
         <is>
-          <t>relefant@mazalaai.com.br</t>
+          <t>cnakata@me.com</t>
         </is>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="inlineStr">
         <is>
-          <t>cnakata@me.com</t>
+          <t>roney@menegasse.com.br</t>
         </is>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="inlineStr">
         <is>
-          <t>roney@menegasse.com.br</t>
+          <t>roberto@mhinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="inlineStr">
         <is>
-          <t>roberto@mhinvestimentos.com.br</t>
+          <t>bruna@milenium.adm.br</t>
         </is>
       </c>
     </row>
     <row r="646">
       <c r="A646" t="inlineStr">
         <is>
-          <t>bruna@milenium.adm.br</t>
+          <t>fabio@milenium.adm.br</t>
         </is>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="inlineStr">
         <is>
-          <t>fabio@milenium.adm.br</t>
+          <t>guilherme@milenium.adm.br</t>
         </is>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="inlineStr">
         <is>
-          <t>guilherme@milenium.adm.br</t>
+          <t>luca@milenium.adm.br</t>
         </is>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="inlineStr">
         <is>
-          <t>luca@milenium.adm.br</t>
+          <t>marcelo@milenium.adm.br</t>
         </is>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="inlineStr">
         <is>
-          <t>marcelo@milenium.adm.br</t>
+          <t>mint@mintcapital.com.br</t>
         </is>
       </c>
     </row>
     <row r="651">
       <c r="A651" t="inlineStr">
         <is>
-          <t>mint@mintcapital.com.br</t>
+          <t>katiadalrovere@neitinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="652">
       <c r="A652" t="inlineStr">
         <is>
-          <t>katiadalrovere@neitinvest.com.br</t>
+          <t>carlosbrennand@norvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="653">
       <c r="A653" t="inlineStr">
         <is>
-          <t>carlosbrennand@norvest.com.br</t>
+          <t>nemer.alias@oaklandinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="654">
       <c r="A654" t="inlineStr">
         <is>
-          <t>nemer.alias@oaklandinvestimentos.com.br</t>
+          <t>wimryan@oasisinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="655">
       <c r="A655" t="inlineStr">
         <is>
-          <t>wimryan@oasisinvest.com.br</t>
+          <t>ony@ocinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="656">
       <c r="A656" t="inlineStr">
         <is>
-          <t>ony@ocinvestimentos.com.br</t>
+          <t>gardenia@operainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="657">
       <c r="A657" t="inlineStr">
         <is>
-          <t>gardenia@operainvestimentos.com</t>
+          <t>mateus@operainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="658">
       <c r="A658" t="inlineStr">
         <is>
-          <t>mateus@operainvestimentos.com</t>
+          <t>melissa@operainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="659">
       <c r="A659" t="inlineStr">
         <is>
-          <t>melissa@operainvestimentos.com</t>
+          <t>renan@orenandutra.com.br</t>
         </is>
       </c>
     </row>
     <row r="660">
       <c r="A660" t="inlineStr">
         <is>
-          <t>renan@orenandutra.com.br</t>
+          <t>leonardo.penedo@penedoinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>leonardo.penedo@penedoinvestimentos.com.br</t>
+          <t>mateus.lovatti@penedoinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="662">
       <c r="A662" t="inlineStr">
         <is>
-          <t>mateus.lovatti@penedoinvestimentos.com.br</t>
+          <t>thiago.silveira@penedoinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="663">
       <c r="A663" t="inlineStr">
         <is>
-          <t>thiago.silveira@penedoinvestimentos.com.br</t>
+          <t>paulo@phpinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="664">
       <c r="A664" t="inlineStr">
         <is>
-          <t>paulo@phpinvestimentos.com.br</t>
+          <t>ian.gadelha@podiuminvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>ian.gadelha@podiuminvest.com.br</t>
+          <t>conversani@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="666">
       <c r="A666" t="inlineStr">
         <is>
-          <t>conversani@premieri.com.br</t>
+          <t>felipe.jaques@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="667">
       <c r="A667" t="inlineStr">
         <is>
-          <t>felipe.jaques@premieri.com.br</t>
+          <t>gabriel.conversani@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="668">
       <c r="A668" t="inlineStr">
         <is>
-          <t>gabriel.conversani@premieri.com.br</t>
+          <t>juliano.bernartti@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="669">
       <c r="A669" t="inlineStr">
         <is>
-          <t>juliano.bernartti@premieri.com.br</t>
+          <t>victor.bernartti@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>victor.bernartti@premieri.com.br</t>
+          <t>wagner.conversani@premieri.com.br</t>
         </is>
       </c>
     </row>
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>wagner.conversani@premieri.com.br</t>
+          <t>dimas@premioinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>dimas@premioinvest.com.br</t>
+          <t>rizaelcio@riale.com.br</t>
         </is>
       </c>
     </row>
     <row r="673">
       <c r="A673" t="inlineStr">
         <is>
-          <t>rizaelcio@riale.com.br</t>
+          <t>rodolfo@rvminvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>rodolfo@rvminvest.com.br</t>
+          <t>jurema.braga@sarkisinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>jurema.braga@sarkisinvest.com.br</t>
+          <t>rodolfo.remy@sarkisinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>rodolfo.remy@sarkisinvest.com.br</t>
+          <t>tom.pessoa@sarkisinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="inlineStr">
         <is>
-          <t>tom.pessoa@sarkisinvest.com.br</t>
+          <t>pedroborges@segmentobsb.com.br</t>
         </is>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="inlineStr">
         <is>
-          <t>pedroborges@segmentobsb.com.br</t>
+          <t>pedroneto@segmentobsb.com.bR</t>
         </is>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="inlineStr">
         <is>
-          <t>pedroneto@segmentobsb.com.bR</t>
+          <t>contato@serpainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="inlineStr">
         <is>
-          <t>contato@serpainvestimentos.com</t>
+          <t>gustavo@serpainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>gustavo@serpainvestimentos.com</t>
+          <t>lucas@serpainvestimentos.com</t>
         </is>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>lucas@serpainvestimentos.com</t>
+          <t>ricardo@sharke.com.br</t>
         </is>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="inlineStr">
         <is>
-          <t>ricardo@sharke.com.br</t>
+          <t>lucasmartins@skyinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="inlineStr">
         <is>
-          <t>lucasmartins@skyinvest.com.br</t>
+          <t>jorny@slrinvestimentos.com.br</t>
         </is>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="inlineStr">
         <is>
-          <t>jorny@slrinvestimentos.com.br</t>
+          <t>jose.bolibioaai@stemaren.com.br</t>
         </is>
       </c>
     </row>
     <row r="686">
       <c r="A686" t="inlineStr">
         <is>
-          <t>jose.bolibioaai@stemaren.com.br</t>
+          <t>tullio@tbfinvest.com.br</t>
         </is>
       </c>
     </row>
     <row r="687">
       <c r="A687" t="inlineStr">
         <is>
-          <t>tullio@tbfinvest.com.br</t>
+          <t>renatangs@terra.com.br</t>
         </is>
       </c>
     </row>
@@ -6211,161 +6211,161 @@
     <row r="826">
       <c r="A826" t="inlineStr">
         <is>
-          <t xml:space="preserve"> comercial@jbninvestimentos.com.br </t>
+          <t xml:space="preserve"> institucional@ewzcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="827">
       <c r="A827" t="inlineStr">
         <is>
-          <t xml:space="preserve"> institucional@ewzcapital.com.br </t>
+          <t xml:space="preserve"> atendimento@engageinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="828">
       <c r="A828" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@engageinvest.com.br </t>
+          <t xml:space="preserve"> fidus@fidusinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="829">
       <c r="A829" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fidus@fidusinvest.com.br </t>
+          <t xml:space="preserve"> pedro@forevercapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="830">
       <c r="A830" t="inlineStr">
         <is>
-          <t xml:space="preserve"> pedro@forevercapital.com.br </t>
+          <t xml:space="preserve"> rodrigo@futureinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="831">
       <c r="A831" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rodrigo@futureinvest.com.br </t>
+          <t xml:space="preserve"> fmg@g2investimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="832">
       <c r="A832" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fmg@g2investimentos.com.br </t>
+          <t xml:space="preserve"> CARDOSO@GENNESYS.COM </t>
         </is>
       </c>
     </row>
     <row r="833">
       <c r="A833" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CARDOSO@GENNESYS.COM </t>
+          <t xml:space="preserve"> Humberto.Vallone@galapagoscapital.com </t>
         </is>
       </c>
     </row>
     <row r="834">
       <c r="A834" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Humberto.Vallone@galapagoscapital.com </t>
+          <t xml:space="preserve"> contato@grcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="835">
       <c r="A835" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@grcapital.com.br </t>
+          <t xml:space="preserve"> rodrigo@gtcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="836">
       <c r="A836" t="inlineStr">
         <is>
-          <t xml:space="preserve"> rodrigo@gtcapital.com.br </t>
+          <t xml:space="preserve"> administrativo@gueltinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="837">
       <c r="A837" t="inlineStr">
         <is>
-          <t xml:space="preserve"> administrativo@gueltinvestimentos.com.br </t>
+          <t xml:space="preserve"> contato@gwminvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="838">
       <c r="A838" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@gwminvest.com.br </t>
+          <t xml:space="preserve"> christianhino@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="839">
       <c r="A839" t="inlineStr">
         <is>
-          <t xml:space="preserve"> christianhino@hotmail.com </t>
+          <t xml:space="preserve"> haus@hausinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="840">
       <c r="A840" t="inlineStr">
         <is>
-          <t xml:space="preserve"> haus@hausinvest.com.br </t>
+          <t xml:space="preserve"> atendimento@hautinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="841">
       <c r="A841" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atendimento@hautinvestimentos.com.br </t>
+          <t xml:space="preserve"> helcio.aguiar@hautinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="842">
       <c r="A842" t="inlineStr">
         <is>
-          <t xml:space="preserve"> helcio.aguiar@hautinvestimentos.com.br </t>
+          <t xml:space="preserve"> integra@integraalianca.com.br </t>
         </is>
       </c>
     </row>
     <row r="843">
       <c r="A843" t="inlineStr">
         <is>
-          <t xml:space="preserve"> integra@integraalianca.com.br </t>
+          <t xml:space="preserve"> reinaldo@integralinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="844">
       <c r="A844" t="inlineStr">
         <is>
-          <t xml:space="preserve"> reinaldo@integralinvest.com.br </t>
+          <t xml:space="preserve"> keliuda@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="845">
       <c r="A845" t="inlineStr">
         <is>
-          <t xml:space="preserve"> keliuda@hotmail.com </t>
+          <t xml:space="preserve"> garcia@itajubainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="846">
       <c r="A846" t="inlineStr">
         <is>
-          <t xml:space="preserve"> garcia@itajubainvestimentos.com.br </t>
+          <t xml:space="preserve"> iwm@iwm.com.br </t>
         </is>
       </c>
     </row>
     <row r="847">
       <c r="A847" t="inlineStr">
         <is>
-          <t xml:space="preserve"> iwm@iwm.com.br </t>
+          <t xml:space="preserve"> contato@jacarandainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="848">
       <c r="A848" t="inlineStr">
         <is>
-          <t xml:space="preserve"> contato@jacarandainvestimentos.com.br </t>
+          <t xml:space="preserve"> comercial@jbninvestimentos.com.br </t>
         </is>
       </c>
     </row>
@@ -7072,308 +7072,308 @@
     <row r="949">
       <c r="A949" t="inlineStr">
         <is>
-          <t xml:space="preserve">trmontenegro@uol.com.br </t>
+          <t xml:space="preserve">debora@allorainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="950">
       <c r="A950" t="inlineStr">
         <is>
-          <t xml:space="preserve">debora@allorainvestimentos.com.br </t>
+          <t xml:space="preserve">allux@alluxinvestimentos.com; ernesto@alluxinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="951">
       <c r="A951" t="inlineStr">
         <is>
-          <t xml:space="preserve">allux@alluxinvestimentos.com; ernesto@alluxinvestimentos.com </t>
+          <t xml:space="preserve">a.latina@terra.com.br </t>
         </is>
       </c>
     </row>
     <row r="952">
       <c r="A952" t="inlineStr">
         <is>
-          <t xml:space="preserve">a.latina@terra.com.br </t>
+          <t xml:space="preserve">fargeti@slw.com.br </t>
         </is>
       </c>
     </row>
     <row r="953">
       <c r="A953" t="inlineStr">
         <is>
-          <t xml:space="preserve">fargeti@slw.com.br </t>
+          <t xml:space="preserve">antoniofgb@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="954">
       <c r="A954" t="inlineStr">
         <is>
-          <t xml:space="preserve">antoniofgb@hotmail.com </t>
+          <t xml:space="preserve">tony@tonycoelho.com.br </t>
         </is>
       </c>
     </row>
     <row r="955">
       <c r="A955" t="inlineStr">
         <is>
-          <t xml:space="preserve">tony@tonycoelho.com.br </t>
+          <t xml:space="preserve">abreu@arrecifeaai.com.br; carlosvalle@arrecifeaai.com.br; matheus@arrecifeaai.com.br; pedro@arrecifeaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="956">
       <c r="A956" t="inlineStr">
         <is>
-          <t xml:space="preserve">abreu@arrecifeaai.com.br; carlosvalle@arrecifeaai.com.br; matheus@arrecifeaai.com.br; pedro@arrecifeaai.com.br </t>
+          <t xml:space="preserve">gereci@bgrcapital.com.br ; rodrigo@bgrcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="957">
       <c r="A957" t="inlineStr">
         <is>
-          <t xml:space="preserve">gereci@bgrcapital.com.br ; rodrigo@bgrcapital.com.br </t>
+          <t xml:space="preserve">jose.valdoir@blackross.com.br; sgiuntini@blackross.com.br </t>
         </is>
       </c>
     </row>
     <row r="958">
       <c r="A958" t="inlineStr">
         <is>
-          <t xml:space="preserve">jose.valdoir@blackross.com.br; sgiuntini@blackross.com.br </t>
+          <t xml:space="preserve">g.caiuby.novaes@uol.com.br </t>
         </is>
       </c>
     </row>
     <row r="959">
       <c r="A959" t="inlineStr">
         <is>
-          <t xml:space="preserve">g.caiuby.novaes@uol.com.br </t>
+          <t xml:space="preserve">gustavoscabral83@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="960">
       <c r="A960" t="inlineStr">
         <is>
-          <t xml:space="preserve">gustavoscabral83@gmail.com </t>
+          <t xml:space="preserve">daniel@calipeinvestimentos.com </t>
         </is>
       </c>
     </row>
     <row r="961">
       <c r="A961" t="inlineStr">
         <is>
-          <t xml:space="preserve">daniel@calipeinvestimentos.com </t>
+          <t xml:space="preserve">ctaphilipp@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="962">
       <c r="A962" t="inlineStr">
         <is>
-          <t xml:space="preserve">ctaphilipp@gmail.com </t>
+          <t xml:space="preserve">administrativo@conquestconsultoria.com </t>
         </is>
       </c>
     </row>
     <row r="963">
       <c r="A963" t="inlineStr">
         <is>
-          <t xml:space="preserve">administrativo@conquestconsultoria.com </t>
+          <t xml:space="preserve">francisco.vaz@dapesinvestimentos.com.br ; alfredo@dapesinvestimentos.com.br; rodrigo@dapesinvestimentos.com.br; joão@dapesinvestimentos.com.br; henrique@dapesinvestimentos.com.br; felipe@dapesinvestimentos.com.br; raul@dapesinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t xml:space="preserve">francisco.vaz@dapesinvestimentos.com.br ; alfredo@dapesinvestimentos.com.br; rodrigo@dapesinvestimentos.com.br; joão@dapesinvestimentos.com.br; henrique@dapesinvestimentos.com.br; felipe@dapesinvestimentos.com.br; raul@dapesinvestimentos.com.br </t>
+          <t xml:space="preserve">denerp.ag@gmail.com  </t>
         </is>
       </c>
     </row>
     <row r="965">
       <c r="A965" t="inlineStr">
         <is>
-          <t xml:space="preserve">denerp.ag@gmail.com  </t>
+          <t xml:space="preserve">sibelle@diamantinainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="966">
       <c r="A966" t="inlineStr">
         <is>
-          <t xml:space="preserve">sibelle@diamantinainvestimentos.com.br </t>
+          <t xml:space="preserve">socios@dnainvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="967">
       <c r="A967" t="inlineStr">
         <is>
-          <t xml:space="preserve">socios@dnainvest.com.br </t>
+          <t xml:space="preserve">henrique@aai.loteinvest.com; fernando@aai.loteinvest.com </t>
         </is>
       </c>
     </row>
     <row r="968">
       <c r="A968" t="inlineStr">
         <is>
-          <t xml:space="preserve">henrique@aai.loteinvest.com; fernando@aai.loteinvest.com </t>
+          <t xml:space="preserve">ctn@egsinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="969">
       <c r="A969" t="inlineStr">
         <is>
-          <t xml:space="preserve">ctn@egsinvestimentos.com.br </t>
+          <t xml:space="preserve">elizabetholivo.bnpp@hotmail.com </t>
         </is>
       </c>
     </row>
     <row r="970">
       <c r="A970" t="inlineStr">
         <is>
-          <t xml:space="preserve">elizabetholivo.bnpp@hotmail.com </t>
+          <t xml:space="preserve">ennardelli@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="971">
       <c r="A971" t="inlineStr">
         <is>
-          <t xml:space="preserve">ennardelli@gmail.com </t>
+          <t xml:space="preserve">isidoriosimoes@atuacaopart.com.br </t>
         </is>
       </c>
     </row>
     <row r="972">
       <c r="A972" t="inlineStr">
         <is>
-          <t xml:space="preserve">jminvestimentos@jotam.com.br </t>
+          <t xml:space="preserve">alexandre.abreu@estruturalinvestimentos.com.br; fernando.zanoli@estruturalinvestimentos.com.br; camila.lessa@estruturalinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="973">
       <c r="A973" t="inlineStr">
         <is>
-          <t xml:space="preserve">isidoriosimoes@atuacaopart.com.br </t>
+          <t xml:space="preserve">gustavo.ribolli@einv.com.br; admilson@einvcom.br; gilberto.gumieri@einv.com.br; </t>
         </is>
       </c>
     </row>
     <row r="974">
       <c r="A974" t="inlineStr">
         <is>
-          <t xml:space="preserve">alexandre.abreu@estruturalinvestimentos.com.br; fernando.zanoli@estruturalinvestimentos.com.br; camila.lessa@estruturalinvestimentos.com.br </t>
+          <t xml:space="preserve">contato@facilitainveste.com.br | julio.basilio@facilitainveste.com.br |rgonzalez@facilitainveste.com.br | leonardo.lewandowski@facilitainveste.com.br | rafael.pianca@facilitainveste.com.br | moacir.arimura@facilitainveste.com.br </t>
         </is>
       </c>
     </row>
     <row r="975">
       <c r="A975" t="inlineStr">
         <is>
-          <t xml:space="preserve">gustavo.ribolli@einv.com.br; admilson@einvcom.br; gilberto.gumieri@einv.com.br; </t>
+          <t xml:space="preserve">marcello.predolin@flapcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="976">
       <c r="A976" t="inlineStr">
         <is>
-          <t xml:space="preserve">contato@facilitainveste.com.br | julio.basilio@facilitainveste.com.br |rgonzalez@facilitainveste.com.br | leonardo.lewandowski@facilitainveste.com.br | rafael.pianca@facilitainveste.com.br | moacir.arimura@facilitainveste.com.br </t>
+          <t xml:space="preserve">flavia.nunnes@nunnesinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="977">
       <c r="A977" t="inlineStr">
         <is>
-          <t xml:space="preserve">marcello.predolin@flapcapital.com.br </t>
+          <t xml:space="preserve">renato.sabino@fmbinvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="978">
       <c r="A978" t="inlineStr">
         <is>
-          <t xml:space="preserve">flavia.nunnes@nunnesinvestimentos.com.br </t>
+          <t xml:space="preserve">fbrant@refraninvest.com.br; carolferreira@refraninvest.com.br </t>
         </is>
       </c>
     </row>
     <row r="979">
       <c r="A979" t="inlineStr">
         <is>
-          <t xml:space="preserve">renato.sabino@fmbinvest.com.br </t>
+          <t xml:space="preserve">eilatinvestimentos@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="980">
       <c r="A980" t="inlineStr">
         <is>
-          <t xml:space="preserve">fbrant@refraninvest.com.br; carolferreira@refraninvest.com.br </t>
+          <t xml:space="preserve">gdias@guideinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="981">
       <c r="A981" t="inlineStr">
         <is>
-          <t xml:space="preserve">eilatinvestimentos@gmail.com </t>
+          <t xml:space="preserve">paulo@goldrock.com.br; </t>
         </is>
       </c>
     </row>
     <row r="982">
       <c r="A982" t="inlineStr">
         <is>
-          <t xml:space="preserve">gdias@guideinvestimentos.com.br </t>
+          <t xml:space="preserve">guilherme.moraes@grmcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="983">
       <c r="A983" t="inlineStr">
         <is>
-          <t xml:space="preserve">paulo@goldrock.com.br; </t>
+          <t xml:space="preserve">gwm@gwmpx.com </t>
         </is>
       </c>
     </row>
     <row r="984">
       <c r="A984" t="inlineStr">
         <is>
-          <t xml:space="preserve">guilherme.moraes@grmcapital.com.br </t>
+          <t xml:space="preserve">luiz@helmanadvisor.com.br </t>
         </is>
       </c>
     </row>
     <row r="985">
       <c r="A985" t="inlineStr">
         <is>
-          <t xml:space="preserve">gwm@gwmpx.com </t>
+          <t xml:space="preserve">luiz@investgroup.com.br; pellin@investigroup.com.br </t>
         </is>
       </c>
     </row>
     <row r="986">
       <c r="A986" t="inlineStr">
         <is>
-          <t xml:space="preserve">luiz@helmanadvisor.com.br </t>
+          <t xml:space="preserve">rsoggia@itajubainvestimentos.com.br ; pbiase@itajubainvestimentos.com.br ; mizael@itajubainvestimentos.com.br ; bqueima@itajubainvestimentos.com.br ; garcia@itajubainvestimentos.com.br ; filipe@itajubainvestimentos.com.br ; agnaldo.andrade@itajubainvestimentos.com.br ; lcamozzato@itajubainvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="987">
       <c r="A987" t="inlineStr">
         <is>
-          <t xml:space="preserve">luiz@investgroup.com.br; pellin@investigroup.com.br </t>
+          <t xml:space="preserve">jacques.abram@abramaai.com.br </t>
         </is>
       </c>
     </row>
     <row r="988">
       <c r="A988" t="inlineStr">
         <is>
-          <t xml:space="preserve">rsoggia@itajubainvestimentos.com.br ; pbiase@itajubainvestimentos.com.br ; mizael@itajubainvestimentos.com.br ; bqueima@itajubainvestimentos.com.br ; garcia@itajubainvestimentos.com.br ; filipe@itajubainvestimentos.com.br ; agnaldo.andrade@itajubainvestimentos.com.br ; lcamozzato@itajubainvestimentos.com.br </t>
+          <t xml:space="preserve">maikel@jacobcapital.com.br </t>
         </is>
       </c>
     </row>
     <row r="989">
       <c r="A989" t="inlineStr">
         <is>
-          <t xml:space="preserve">jacques.abram@abramaai.com.br </t>
+          <t xml:space="preserve">jbatistaautonomosjosecarlos@gmail.com; jbatistaautonomos.gabriel@gmail.com </t>
         </is>
       </c>
     </row>
     <row r="990">
       <c r="A990" t="inlineStr">
         <is>
-          <t xml:space="preserve">maikel@jacobcapital.com.br </t>
+          <t xml:space="preserve">leon@jlvinvestimentos.com.br </t>
         </is>
       </c>
     </row>
     <row r="991">
       <c r="A991" t="inlineStr">
         <is>
-          <t xml:space="preserve">jbatistaautonomosjosecarlos@gmail.com; jbatistaautonomos.gabriel@gmail.com </t>
+          <t xml:space="preserve">jminvestimentos@jotam.com.br </t>
         </is>
       </c>
     </row>
     <row r="992">
       <c r="A992" t="inlineStr">
         <is>
-          <t xml:space="preserve">leon@jlvinvestimentos.com.br </t>
+          <t xml:space="preserve">trmontenegro@uol.com.br </t>
         </is>
       </c>
     </row>

</xml_diff>